<commit_message>
several changes for storage testing; Vangelis RF_CMD example; multiple currencies for the same attribute.
</commit_message>
<xml_diff>
--- a/BY_Trans.xlsx
+++ b/BY_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEE6359-4456-4A9C-AACD-EC73B50733A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AB0A05-F864-453B-854B-3E341A36A722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="1335" windowWidth="18135" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4815" yWindow="1410" windowWidth="20040" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NCAP_BND" sheetId="20" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -89,9 +89,6 @@
     <t>TimeSlice</t>
   </si>
   <si>
-    <t>LimType</t>
-  </si>
-  <si>
     <t>Attribute</t>
   </si>
   <si>
@@ -195,6 +192,18 @@
   </si>
   <si>
     <t>INDELC</t>
+  </si>
+  <si>
+    <t>COM_AGG</t>
+  </si>
+  <si>
+    <t>???CO2,-TOTCO2</t>
+  </si>
+  <si>
+    <t>other_indexes</t>
+  </si>
+  <si>
+    <t>TOTCO2</t>
   </si>
 </sst>
 </file>
@@ -722,7 +731,7 @@
   <dimension ref="B3:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -734,7 +743,7 @@
   <sheetData>
     <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
@@ -755,51 +764,51 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -808,58 +817,72 @@
         <v>2</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>21</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>22</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>23</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>24</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>25</v>
-      </c>
-      <c r="K13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" t="s">
         <v>30</v>
-      </c>
-      <c r="H14" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
@@ -869,57 +892,57 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
         <v>19</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>20</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>21</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>22</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>23</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>24</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>25</v>
       </c>
-      <c r="L18" t="s">
-        <v>26</v>
-      </c>
       <c r="M18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>2005</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19">
         <v>0.5</v>
@@ -927,13 +950,13 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>2006</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20">
         <v>0.51</v>
@@ -941,13 +964,13 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>2007</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21">
         <v>0.52</v>
@@ -955,13 +978,13 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>2008</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22">
         <v>0.53</v>
@@ -969,13 +992,13 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>2009</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F23">
         <v>0.54</v>
@@ -983,13 +1006,13 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>2010</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F24">
         <v>0.55000000000000004</v>
@@ -997,13 +1020,13 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>2011</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F25">
         <v>0.56000000000000005</v>
@@ -1011,16 +1034,16 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UDCG as commodi name case; testing retirement
</commit_message>
<xml_diff>
--- a/BY_Trans.xlsx
+++ b/BY_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AB0A05-F864-453B-854B-3E341A36A722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36C470F-1A73-4DF1-9E8B-8E6D47CB4011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="1410" windowWidth="20040" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NCAP_BND" sheetId="20" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>TOTCO2</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
@@ -730,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -834,6 +837,17 @@
         <v>38</v>
       </c>
     </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <v>2005</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
CPX example; case for UD set in BY_Trans, which doesn't work if only BY_Trans is synced
</commit_message>
<xml_diff>
--- a/BY_Trans.xlsx
+++ b/BY_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36C470F-1A73-4DF1-9E8B-8E6D47CB4011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B12969-683B-46A3-9847-BDFD187091B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1695" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NCAP_BND" sheetId="20" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -179,9 +179,6 @@
     <t>ELCCOA</t>
   </si>
   <si>
-    <t>ELCGAS</t>
-  </si>
-  <si>
     <t>STG_SIFT</t>
   </si>
   <si>
@@ -207,6 +204,12 @@
   </si>
   <si>
     <t>END</t>
+  </si>
+  <si>
+    <t>Pset_set</t>
+  </si>
+  <si>
+    <t>ELEGAS</t>
   </si>
 </sst>
 </file>
@@ -734,7 +737,7 @@
   <dimension ref="B3:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -767,7 +770,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>2</v>
@@ -825,21 +828,21 @@
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>2005</v>
@@ -912,7 +915,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
@@ -942,10 +945,10 @@
         <v>14</v>
       </c>
       <c r="N18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
@@ -956,7 +959,7 @@
         <v>2005</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F19">
         <v>0.5</v>
@@ -970,7 +973,7 @@
         <v>2006</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F20">
         <v>0.51</v>
@@ -984,7 +987,7 @@
         <v>2007</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F21">
         <v>0.52</v>
@@ -998,7 +1001,7 @@
         <v>2008</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F22">
         <v>0.53</v>
@@ -1012,7 +1015,7 @@
         <v>2009</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F23">
         <v>0.54</v>
@@ -1026,7 +1029,7 @@
         <v>2010</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F24">
         <v>0.55000000000000004</v>
@@ -1040,7 +1043,7 @@
         <v>2011</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F25">
         <v>0.56000000000000005</v>
@@ -1048,16 +1051,16 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
case: VT_ values come from DINS in BY_Trans - DINS values should survive for all regions.
</commit_message>
<xml_diff>
--- a/BY_Trans.xlsx
+++ b/BY_Trans.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B12969-683B-46A3-9847-BDFD187091B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939EDF1C-DE11-4450-A552-844077943332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1695" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28898" yWindow="1643" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NCAP_BND" sheetId="20" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="21" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -210,6 +211,21 @@
   </si>
   <si>
     <t>ELEGAS</t>
+  </si>
+  <si>
+    <t>~TFM_DINS-TS</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>act_cost</t>
+  </si>
+  <si>
+    <t>ELCNENUC00</t>
   </si>
 </sst>
 </file>
@@ -414,9 +430,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -454,9 +470,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,26 +505,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,26 +540,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -736,23 +718,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -765,7 +747,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -812,7 +794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>16</v>
       </c>
@@ -826,7 +808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>39</v>
       </c>
@@ -840,7 +822,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>40</v>
       </c>
@@ -851,12 +833,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -888,7 +870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -902,12 +884,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -951,7 +933,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>27</v>
       </c>
@@ -965,7 +947,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>27</v>
       </c>
@@ -979,7 +961,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>27</v>
       </c>
@@ -993,7 +975,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>27</v>
       </c>
@@ -1007,7 +989,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -1021,7 +1003,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>27</v>
       </c>
@@ -1035,7 +1017,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>27</v>
       </c>
@@ -1049,7 +1031,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
@@ -1067,4 +1049,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C971E9-0AD6-442D-B65E-6F6801329DEC}">
+  <dimension ref="B6:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8">
+        <v>0.44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added cases for handling year2 dim in fetch queries.
</commit_message>
<xml_diff>
--- a/BY_Trans.xlsx
+++ b/BY_Trans.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6983FD8-F182-42DA-8808-EB0283CE4E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640561A6-902E-4B94-B3BE-C239BC43ABBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1808" yWindow="1808" windowWidth="21600" windowHeight="12682" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NCAP_BND" sheetId="20" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="21" r:id="rId2"/>
+    <sheet name="year2 dimension" sheetId="22" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -259,6 +260,27 @@
   </si>
   <si>
     <t>Gas_invalid</t>
+  </si>
+  <si>
+    <t>~TFM_MIG</t>
+  </si>
+  <si>
+    <t>CUM</t>
+  </si>
+  <si>
+    <t>year2</t>
+  </si>
+  <si>
+    <t>BOH-2030</t>
+  </si>
+  <si>
+    <t>*COA*</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>*.5</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C971E9-0AD6-442D-B65E-6F6801329DEC}">
   <dimension ref="A6:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1393,4 +1415,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001761B2-0FD6-4D51-B74C-BBF5F040EA39}">
+  <dimension ref="B3:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>